<commit_message>
Added Scaled Tanh activation.
</commit_message>
<xml_diff>
--- a/data/Activation Function Tests.xlsx
+++ b/data/Activation Function Tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\NetBeansProjects\OptimizationToolkit\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17235" windowHeight="8265"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="17232" windowHeight="8268"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>tanh</t>
   </si>
@@ -76,13 +81,16 @@
   </si>
   <si>
     <t>100000</t>
+  </si>
+  <si>
+    <t>scaledTanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +136,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +222,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +257,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,25 +433,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -441,7 +459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -469,7 +487,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -501,7 +519,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -535,7 +553,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,34 +593,28 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>78.821899999999999</v>
+        <v>45.471400000000003</v>
       </c>
       <c r="C6" s="1">
-        <v>31.435400000000001</v>
+        <v>41.372500000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>52.2179</v>
+        <v>17.931999999999999</v>
       </c>
       <c r="E6" s="1">
-        <v>86.006399999999999</v>
+        <v>13.785600000000001</v>
       </c>
       <c r="F6" s="1">
-        <v>40.083100000000002</v>
-      </c>
-      <c r="G6" s="1">
-        <v>16.6281</v>
-      </c>
-      <c r="H6" s="1">
-        <v>100</v>
-      </c>
-      <c r="I6" s="1">
-        <v>4.3220999999999998</v>
-      </c>
+        <v>11.2369</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -615,33 +627,33 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>45.104900000000001</v>
+        <v>78.821899999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>40.639699999999998</v>
+        <v>31.435400000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>44.557499999999997</v>
+        <v>52.2179</v>
       </c>
       <c r="E7" s="1">
-        <v>40.796700000000001</v>
+        <v>86.006399999999999</v>
       </c>
       <c r="F7" s="1">
-        <v>11.534000000000001</v>
+        <v>40.083100000000002</v>
       </c>
       <c r="G7" s="1">
-        <v>5.0907099999999996</v>
+        <v>16.6281</v>
       </c>
       <c r="H7" s="1">
-        <v>40.6404</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1">
-        <v>5.8700599999999996</v>
+        <v>4.3220999999999998</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -655,33 +667,33 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
-        <v>39.834899999999998</v>
+        <v>45.104900000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>29.549199999999999</v>
+        <v>40.639699999999998</v>
       </c>
       <c r="D8" s="1">
-        <v>11.5769</v>
+        <v>44.557499999999997</v>
       </c>
       <c r="E8" s="1">
-        <v>57.689900000000002</v>
+        <v>40.796700000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>10.3627</v>
+        <v>11.534000000000001</v>
       </c>
       <c r="G8" s="1">
-        <v>4.6416899999999996</v>
+        <v>5.0907099999999996</v>
       </c>
       <c r="H8" s="1">
-        <v>100.006</v>
+        <v>40.6404</v>
       </c>
       <c r="I8" s="1">
-        <v>100.16500000000001</v>
+        <v>5.8700599999999996</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -695,33 +707,33 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>65.286500000000004</v>
+        <v>39.834899999999998</v>
       </c>
       <c r="C9" s="1">
-        <v>34.265000000000001</v>
+        <v>29.549199999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>25.001799999999999</v>
+        <v>11.5769</v>
       </c>
       <c r="E9" s="1">
-        <v>39.966299999999997</v>
+        <v>57.689900000000002</v>
       </c>
       <c r="F9" s="1">
-        <v>34.349600000000002</v>
+        <v>10.3627</v>
       </c>
       <c r="G9" s="1">
-        <v>5.1957599999999999</v>
+        <v>4.6416899999999996</v>
       </c>
       <c r="H9" s="1">
-        <v>99.990899999999996</v>
+        <v>100.006</v>
       </c>
       <c r="I9" s="1">
-        <v>5.5618699999999999</v>
+        <v>100.16500000000001</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -735,33 +747,33 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>42.698300000000003</v>
+        <v>65.286500000000004</v>
       </c>
       <c r="C10" s="1">
-        <v>39.359400000000001</v>
+        <v>34.265000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>15.4312</v>
+        <v>25.001799999999999</v>
       </c>
       <c r="E10" s="1">
-        <v>13.162800000000001</v>
+        <v>39.966299999999997</v>
       </c>
       <c r="F10" s="1">
-        <v>11.1907</v>
+        <v>34.349600000000002</v>
       </c>
       <c r="G10" s="1">
-        <v>4.1717899999999997</v>
+        <v>5.1957599999999999</v>
       </c>
       <c r="H10" s="1">
-        <v>9.7992399999999993</v>
+        <v>99.990899999999996</v>
       </c>
       <c r="I10" s="1">
-        <v>5.4263300000000001</v>
+        <v>5.5618699999999999</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -775,33 +787,33 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>47.731200000000001</v>
+        <v>42.698300000000003</v>
       </c>
       <c r="C11" s="1">
-        <v>42.180199999999999</v>
+        <v>39.359400000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>14.295400000000001</v>
+        <v>15.4312</v>
       </c>
       <c r="E11" s="1">
-        <v>12.4049</v>
+        <v>13.162800000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>11.832000000000001</v>
+        <v>11.1907</v>
       </c>
       <c r="G11" s="1">
-        <v>4.3899800000000004</v>
+        <v>4.1717899999999997</v>
       </c>
       <c r="H11" s="1">
-        <v>5.1714000000000002</v>
+        <v>9.7992399999999993</v>
       </c>
       <c r="I11" s="1">
-        <v>5.8007799999999996</v>
+        <v>5.4263300000000001</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -814,6 +826,46 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>47.731200000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42.180199999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>14.295400000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.4049</v>
+      </c>
+      <c r="F12" s="1">
+        <v>11.832000000000001</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4.3899800000000004</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5.1714000000000002</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5.8007799999999996</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -829,24 +881,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added demos directory for demos/test drivers. Finished test with scaledTanhActivation. Results file updated.
</commit_message>
<xml_diff>
--- a/data/Activation Function Tests.xlsx
+++ b/data/Activation Function Tests.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\NetBeansProjects\OptimizationToolkit\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="48" windowWidth="17232" windowHeight="8268"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17235" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,10 +217,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,7 +251,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,25 +426,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -459,7 +452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -487,7 +480,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -519,7 +512,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -553,7 +546,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,7 +586,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -612,9 +605,15 @@
       <c r="F6" s="1">
         <v>11.2369</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="G6" s="1">
+        <v>4.5423</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6.9443799999999998</v>
+      </c>
+      <c r="I6" s="1">
+        <v>6.2509300000000003</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -627,7 +626,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -667,7 +666,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -707,7 +706,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -747,7 +746,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -787,7 +786,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -827,7 +826,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -881,24 +880,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>